<commit_message>
shopping cart page complete module push
</commit_message>
<xml_diff>
--- a/resources/ExcelsheetData/QuickCartData/FileUploadTestData.xlsx
+++ b/resources/ExcelsheetData/QuickCartData/FileUploadTestData.xlsx
@@ -528,7 +528,7 @@
   <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:C7"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,49 +560,31 @@
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -610,256 +592,160 @@
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="2"/>
-      <c r="D8">
-        <v>1</v>
-      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D11">
-        <v>1</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D12">
-        <v>1</v>
-      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D14">
-        <v>1</v>
-      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D39">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>